<commit_message>
chore: fixed commission report headers; add: added missing headers in reports; fix: fixed member and user leave apis
</commit_message>
<xml_diff>
--- a/resources/excel/CommissionWorkbook.xlsx
+++ b/resources/excel/CommissionWorkbook.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="60">
   <si>
     <t>commissions_summary_list</t>
   </si>
@@ -132,6 +132,18 @@
     <t>commission</t>
   </si>
   <si>
+    <t>external_id</t>
+  </si>
+  <si>
+    <t>#ioy2fcf</t>
+  </si>
+  <si>
+    <t>utm_id</t>
+  </si>
+  <si>
+    <t>wvninnewn</t>
+  </si>
+  <si>
     <t>utm_source</t>
   </si>
   <si>
@@ -144,10 +156,31 @@
     <t>social</t>
   </si>
   <si>
+    <t>utm_campaign</t>
+  </si>
+  <si>
+    <t>fireship</t>
+  </si>
+  <si>
+    <t>utm_term</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>utm_content</t>
+  </si>
+  <si>
+    <t>logolink</t>
+  </si>
+  <si>
     <t>purchase_commissions_table</t>
   </si>
   <si>
     <t>purchase_id</t>
+  </si>
+  <si>
+    <t>purchase_date</t>
   </si>
   <si>
     <t>29e2b940-7413-4e9a-89ce-bace8bfc6f3b</t>
@@ -258,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -289,6 +322,15 @@
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -976,25 +1018,40 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="10"/>
+      <c r="C8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="12"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="12" t="s">
         <v>40</v>
       </c>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
+      <c r="P8" s="13"/>
+      <c r="Q8" s="13"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="13"/>
+      <c r="T8" s="13"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="13"/>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
@@ -1006,37 +1063,155 @@
       <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="10" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="K10" s="12"/>
+      <c r="A10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="7" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="A12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="14"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="K18" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1062,7 +1237,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1112,7 +1287,7 @@
     </row>
     <row r="3">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>13</v>
@@ -1135,7 +1310,7 @@
     </row>
     <row r="4">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>13</v>
@@ -1149,16 +1324,14 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
-      <c r="J4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>45</v>
+      <c r="J4" s="7"/>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="7" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>13</v>
@@ -1172,37 +1345,37 @@
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7" t="s">
-        <v>47</v>
+      <c r="J5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="7" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="7">
-        <v>0.01</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="7">
-        <v>980.0</v>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>13</v>
@@ -1210,8 +1383,8 @@
       <c r="C7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="10">
-        <v>0.0</v>
+      <c r="D7" s="7">
+        <v>0.01</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -1219,72 +1392,269 @@
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
-      <c r="K7" s="10">
-        <v>91.0</v>
+      <c r="K7" s="7">
+        <v>980.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="10"/>
+        <v>24</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.0</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8"/>
-      <c r="K8" s="10" t="s">
-        <v>40</v>
+      <c r="K8" s="10">
+        <v>91.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="7"/>
+      <c r="C9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="12"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
+      <c r="P9" s="13"/>
+      <c r="Q9" s="13"/>
+      <c r="R9" s="13"/>
+      <c r="S9" s="13"/>
+      <c r="T9" s="13"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="13"/>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="K10" s="12"/>
-    </row>
     <row r="11">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
+      <c r="A11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="12"/>
-      <c r="K11" s="12"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
     </row>
     <row r="12">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>14</v>
+      </c>
       <c r="D12" s="12"/>
-      <c r="K12" s="12"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>